<commit_message>
Sinh Vien Improt-- return error not done yet
</commit_message>
<xml_diff>
--- a/Web_Datamining/Web_Datamining.Web/ExcelFormat/Students.xlsx
+++ b/Web_Datamining/Web_Datamining.Web/ExcelFormat/Students.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\DACN\Web_Datamining_Hutech\Web_Datamining\Web_Datamining.Web\ExcelFormat\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -356,7 +356,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>